<commit_message>
Game pong following evaluations done: only_semantic_smells, only_syntactic_smells. All smells evaluation hotfix.
</commit_message>
<xml_diff>
--- a/evaluations/GPT/2025-04-05_094619/pong/all_smells_01/evaluation.xlsx
+++ b/evaluations/GPT/2025-04-05_094619/pong/all_smells_01/evaluation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>1.4</t>
+  </si>
+  <si>
+    <t>2.5.1</t>
   </si>
   <si>
     <t>logical_inconsistencies</t>
@@ -616,9 +619,11 @@
         <v>16</v>
       </c>
       <c r="F11" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="G11" s="2"/>
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -631,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <v>1.0</v>
@@ -652,16 +657,16 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1">
         <v>0.0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1">
         <v>0.0</v>
@@ -678,16 +683,16 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1">
         <v>0.0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1">
         <v>1.0</v>
@@ -705,7 +710,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1">
         <v>1.0</v>
@@ -750,16 +755,16 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1">
         <v>0.0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1">
         <v>0.0</v>
@@ -776,10 +781,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1">
         <v>0.0</v>
@@ -802,10 +807,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1">
         <v>0.0</v>
@@ -831,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1">
         <v>1.0</v>
@@ -841,7 +846,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -855,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="1">
         <v>0.0</v>
@@ -875,7 +880,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -886,7 +891,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3">
         <f>SUM(F2:F21)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>

</xml_diff>